<commit_message>
Allow to continuously add file names in one instance
</commit_message>
<xml_diff>
--- a/test.xlsx
+++ b/test.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="B1:B13"/>
+  <dimension ref="B1:B25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -512,6 +512,90 @@
         </is>
       </c>
     </row>
+    <row r="14">
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>CV_Santiago</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>CV_SantiagoRodriguez</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>CV_SantiagoRodriguez</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>CV_SRF</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>GeneralCV</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>LACCD_CL</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>Resume_Santiago</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>RodriguezFlores_Santiago_Resume</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>RodriguezSantiago_Resume2021 - Copy</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>SBCC_Resume</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>SMC_CL</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>tax2022</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>